<commit_message>
Dap an bai 28
</commit_message>
<xml_diff>
--- a/data_sample/data_2_3/crosstab2.xlsx
+++ b/data_sample/data_2_3/crosstab2.xlsx
@@ -198,6 +198,48 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>494640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14760</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>113760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3649680" y="1476360"/>
+          <a:ext cx="4228200" cy="2828160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -206,7 +248,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,5 +591,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>